<commit_message>
Descriptive statistics for Pixel 5 updated
</commit_message>
<xml_diff>
--- a/Analysis/Pixel5/curated_data/Descriptive Statistics for Pixel 5.xlsx
+++ b/Analysis/Pixel5/curated_data/Descriptive Statistics for Pixel 5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02098C82-1656-4FA6-B291-3E116EC3ED1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC5ED80-CE2B-451E-A1A3-B08EA28EE291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="2055" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -182,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,10 +201,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -428,7 +425,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -500,7 +497,8 @@
         <v>7</v>
       </c>
       <c r="B4" s="8">
-        <v>4.705E-3</v>
+        <f>0.004705*1000</f>
+        <v>4.7050000000000001</v>
       </c>
       <c r="C4" s="3">
         <v>113.48</v>
@@ -508,8 +506,9 @@
       <c r="D4" s="3">
         <v>12.519600000000001</v>
       </c>
-      <c r="E4" s="9">
-        <v>2.8219272000000002E-3</v>
+      <c r="E4" s="8">
+        <f>0.0028219272*1000</f>
+        <v>2.8219272000000002</v>
       </c>
       <c r="F4" s="3">
         <v>58.92</v>
@@ -517,8 +516,9 @@
       <c r="G4" s="3">
         <v>12.43918</v>
       </c>
-      <c r="H4" s="9">
-        <v>3.9976932000000001E-3</v>
+      <c r="H4" s="8">
+        <f>0.0039976932*1000</f>
+        <v>3.9976932000000001</v>
       </c>
       <c r="I4" s="3">
         <v>55.04</v>
@@ -531,8 +531,9 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9">
-        <v>4.5644119000000007E-3</v>
+      <c r="B5" s="8">
+        <f>0.0045644119*1000</f>
+        <v>4.5644118999999996</v>
       </c>
       <c r="C5" s="3">
         <v>117.4503867</v>
@@ -540,8 +541,9 @@
       <c r="D5" s="3">
         <v>2.2593019999999999</v>
       </c>
-      <c r="E5" s="9">
-        <v>1.1199818E-3</v>
+      <c r="E5" s="8">
+        <f>0.0011199818*1000</f>
+        <v>1.1199817999999999</v>
       </c>
       <c r="F5" s="3">
         <v>78.57423</v>
@@ -549,8 +551,9 @@
       <c r="G5" s="3">
         <v>2.2124069999999998</v>
       </c>
-      <c r="H5" s="9">
-        <v>1.7048259000000002E-3</v>
+      <c r="H5" s="8">
+        <f>0.0017048259*1000</f>
+        <v>1.7048258999999999</v>
       </c>
       <c r="I5" s="3">
         <v>136.7569</v>
@@ -563,8 +566,9 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9">
-        <v>2.17759062E-2</v>
+      <c r="B6" s="8">
+        <f>0.0217759062*1000</f>
+        <v>21.775906200000001</v>
       </c>
       <c r="C6" s="3">
         <v>552</v>
@@ -572,8 +576,9 @@
       <c r="D6" s="3">
         <v>18.648150000000001</v>
       </c>
-      <c r="E6" s="9">
-        <v>6.3845291000000004E-3</v>
+      <c r="E6" s="8">
+        <f>0.0063845291*1000</f>
+        <v>6.3845291</v>
       </c>
       <c r="F6" s="3">
         <v>378</v>
@@ -581,8 +586,9 @@
       <c r="G6" s="3">
         <v>18.44763</v>
       </c>
-      <c r="H6" s="9">
-        <v>8.7333419000000002E-3</v>
+      <c r="H6" s="8">
+        <f>0.0087333419*1000</f>
+        <v>8.733341900000001</v>
       </c>
       <c r="I6" s="3">
         <v>673</v>
@@ -595,8 +601,9 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9">
-        <v>4.7509563000000003E-3</v>
+      <c r="B7" s="8">
+        <f>0.0047509563*1000</f>
+        <v>4.7509563000000004</v>
       </c>
       <c r="C7" s="3">
         <v>127</v>
@@ -604,8 +611,9 @@
       <c r="D7" s="3">
         <v>13.05832</v>
       </c>
-      <c r="E7" s="9">
-        <v>2.8627958999999999E-3</v>
+      <c r="E7" s="8">
+        <f>0.0028627959*1000</f>
+        <v>2.8627959000000001</v>
       </c>
       <c r="F7" s="3">
         <v>43</v>
@@ -613,8 +621,9 @@
       <c r="G7" s="3">
         <v>12.900219999999999</v>
       </c>
-      <c r="H7" s="9">
-        <v>4.5995100000000002E-3</v>
+      <c r="H7" s="8">
+        <f>0.00459951*1000</f>
+        <v>4.5995100000000004</v>
       </c>
       <c r="I7" s="3">
         <v>18</v>
@@ -627,8 +636,9 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9">
-        <v>3.5358382E-3</v>
+      <c r="B8" s="8">
+        <f>0.0035358382*1000</f>
+        <v>3.5358382000000002</v>
       </c>
       <c r="C8" s="3">
         <v>74</v>
@@ -636,8 +646,9 @@
       <c r="D8" s="3">
         <v>11.44117</v>
       </c>
-      <c r="E8" s="9">
-        <v>2.3974599999999997E-3</v>
+      <c r="E8" s="8">
+        <f>0.00239746*1000</f>
+        <v>2.3974600000000001</v>
       </c>
       <c r="F8" s="3">
         <v>36</v>
@@ -645,8 +656,9 @@
       <c r="G8" s="3">
         <v>11.355840000000001</v>
       </c>
-      <c r="H8" s="9">
-        <v>3.4524217E-3</v>
+      <c r="H8" s="8">
+        <f>0.0034524217*1000</f>
+        <v>3.4524216999999999</v>
       </c>
       <c r="I8" s="3">
         <v>14</v>
@@ -659,8 +671,9 @@
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="9">
-        <v>2.4074307000000001E-3</v>
+      <c r="B9" s="8">
+        <f>0.0024074307*1000</f>
+        <v>2.4074306999999999</v>
       </c>
       <c r="C9" s="3">
         <v>45</v>
@@ -668,8 +681,9 @@
       <c r="D9" s="3">
         <v>10.950670000000001</v>
       </c>
-      <c r="E9" s="9">
-        <v>2.2949296E-3</v>
+      <c r="E9" s="8">
+        <f>0.0022949296*1000</f>
+        <v>2.2949296000000001</v>
       </c>
       <c r="F9" s="3">
         <v>29</v>
@@ -677,8 +691,9 @@
       <c r="G9" s="3">
         <v>10.94439</v>
       </c>
-      <c r="H9" s="9">
-        <v>2.7690735000000001E-3</v>
+      <c r="H9" s="8">
+        <f>0.0027690735*1000</f>
+        <v>2.7690735000000002</v>
       </c>
       <c r="I9" s="3">
         <v>10</v>
@@ -691,8 +706,9 @@
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="9">
-        <v>1.8092166E-3</v>
+      <c r="B10" s="8">
+        <f>0.0018092166*1000</f>
+        <v>1.8092166000000001</v>
       </c>
       <c r="C10" s="3">
         <v>10</v>
@@ -700,8 +716,9 @@
       <c r="D10" s="3">
         <v>10.785080000000001</v>
       </c>
-      <c r="E10" s="9">
-        <v>1.6388099000000001E-3</v>
+      <c r="E10" s="8">
+        <f>0.0016388099*1000</f>
+        <v>1.6388099</v>
       </c>
       <c r="F10" s="3">
         <v>14</v>
@@ -709,8 +726,9 @@
       <c r="G10" s="3">
         <v>10.80335</v>
       </c>
-      <c r="H10" s="9">
-        <v>1.8045769000000001E-3</v>
+      <c r="H10" s="8">
+        <f>0.0018045769*1000</f>
+        <v>1.8045769</v>
       </c>
       <c r="I10" s="3">
         <v>6</v>
@@ -797,8 +815,9 @@
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="9">
-        <v>6.1703769999999995E-3</v>
+      <c r="B15" s="8">
+        <f>0.006170377*1000</f>
+        <v>6.1703770000000002</v>
       </c>
       <c r="C15" s="3">
         <v>149.19999999999999</v>
@@ -806,8 +825,9 @@
       <c r="D15" s="3">
         <v>11.147880000000001</v>
       </c>
-      <c r="E15" s="9">
-        <v>2.6569109999999996E-3</v>
+      <c r="E15" s="8">
+        <f>0.002656911*1000</f>
+        <v>2.656911</v>
       </c>
       <c r="F15" s="3">
         <v>104.32</v>
@@ -815,8 +835,9 @@
       <c r="G15" s="3">
         <v>11.16816</v>
       </c>
-      <c r="H15" s="9">
-        <v>4.2586686000000004E-3</v>
+      <c r="H15" s="8">
+        <f>0.0042586686*1000</f>
+        <v>4.2586686</v>
       </c>
       <c r="I15" s="3">
         <v>90.84</v>
@@ -829,8 +850,9 @@
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="9">
-        <v>2.2587786000000001E-3</v>
+      <c r="B16" s="8">
+        <f>0.0022587786*1000</f>
+        <v>2.2587786000000003</v>
       </c>
       <c r="C16" s="3">
         <v>109.00344029999999</v>
@@ -838,8 +860,9 @@
       <c r="D16" s="3">
         <v>0.311672</v>
       </c>
-      <c r="E16" s="9">
-        <v>5.8422770000000001E-4</v>
+      <c r="E16" s="8">
+        <f>0.0005842277*1000</f>
+        <v>0.58422770000000002</v>
       </c>
       <c r="F16" s="3">
         <v>101.6857</v>
@@ -847,8 +870,9 @@
       <c r="G16" s="3">
         <v>0.32464599999999999</v>
       </c>
-      <c r="H16" s="9">
-        <v>4.2095557E-3</v>
+      <c r="H16" s="8">
+        <f>0.0042095557*1000</f>
+        <v>4.2095557000000001</v>
       </c>
       <c r="I16" s="3">
         <v>149.04580000000001</v>
@@ -861,8 +885,9 @@
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="9">
-        <v>1.2115265599999999E-2</v>
+      <c r="B17" s="8">
+        <f>0.0121152656*1000</f>
+        <v>12.115265599999999</v>
       </c>
       <c r="C17" s="3">
         <v>532</v>
@@ -870,8 +895,9 @@
       <c r="D17" s="3">
         <v>11.773849999999999</v>
       </c>
-      <c r="E17" s="9">
-        <v>3.8534959999999997E-3</v>
+      <c r="E17" s="8">
+        <f>0.003853496*1000</f>
+        <v>3.8534960000000003</v>
       </c>
       <c r="F17" s="3">
         <v>460</v>
@@ -879,8 +905,9 @@
       <c r="G17" s="3">
         <v>11.81274</v>
       </c>
-      <c r="H17" s="9">
-        <v>2.3031765799999999E-2</v>
+      <c r="H17" s="8">
+        <f>0.0230317658*1000</f>
+        <v>23.031765799999999</v>
       </c>
       <c r="I17" s="3">
         <v>750</v>
@@ -893,8 +920,9 @@
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="9">
-        <v>6.8265456E-3</v>
+      <c r="B18" s="8">
+        <f>0.0068265456*1000</f>
+        <v>6.8265456000000002</v>
       </c>
       <c r="C18" s="3">
         <v>185</v>
@@ -902,8 +930,9 @@
       <c r="D18" s="3">
         <v>11.381819999999999</v>
       </c>
-      <c r="E18" s="9">
-        <v>3.0935058000000001E-3</v>
+      <c r="E18" s="8">
+        <f>0.0030935058*1000</f>
+        <v>3.0935058</v>
       </c>
       <c r="F18" s="3">
         <v>95</v>
@@ -911,8 +940,9 @@
       <c r="G18" s="3">
         <v>11.4132</v>
       </c>
-      <c r="H18" s="9">
-        <v>4.2487013999999998E-3</v>
+      <c r="H18" s="8">
+        <f>0.0042487014*1000</f>
+        <v>4.2487013999999999</v>
       </c>
       <c r="I18" s="3">
         <v>87</v>
@@ -925,8 +955,9 @@
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="9">
-        <v>5.4967423999999999E-3</v>
+      <c r="B19" s="8">
+        <f>0.0054967424*1000</f>
+        <v>5.4967423999999996</v>
       </c>
       <c r="C19" s="3">
         <v>118</v>
@@ -934,8 +965,9 @@
       <c r="D19" s="3">
         <v>11.014139999999999</v>
       </c>
-      <c r="E19" s="9">
-        <v>2.3973196E-3</v>
+      <c r="E19" s="8">
+        <f>0.0023973196*1000</f>
+        <v>2.3973195999999999</v>
       </c>
       <c r="F19" s="3">
         <v>66</v>
@@ -943,8 +975,9 @@
       <c r="G19" s="3">
         <v>11.04735</v>
       </c>
-      <c r="H19" s="9">
-        <v>3.0870698000000003E-3</v>
+      <c r="H19" s="8">
+        <f>0.0030870698*1000</f>
+        <v>3.0870697999999996</v>
       </c>
       <c r="I19" s="3">
         <v>43</v>
@@ -957,8 +990,9 @@
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="9">
-        <v>4.8682335000000002E-3</v>
+      <c r="B20" s="8">
+        <f>0.0048682335*1000</f>
+        <v>4.8682335000000005</v>
       </c>
       <c r="C20" s="3">
         <v>74</v>
@@ -966,8 +1000,9 @@
       <c r="D20" s="3">
         <v>10.885680000000001</v>
       </c>
-      <c r="E20" s="9">
-        <v>2.1722160999999999E-3</v>
+      <c r="E20" s="8">
+        <f>0.0021722161*1000</f>
+        <v>2.1722161</v>
       </c>
       <c r="F20" s="3">
         <v>56</v>
@@ -975,8 +1010,9 @@
       <c r="G20" s="3">
         <v>10.89498</v>
       </c>
-      <c r="H20" s="9">
-        <v>2.4284689999999999E-3</v>
+      <c r="H20" s="8">
+        <f>0.002428469*1000</f>
+        <v>2.4284689999999998</v>
       </c>
       <c r="I20" s="3">
         <v>24</v>
@@ -989,8 +1025,9 @@
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="9">
-        <v>2.1708051000000001E-3</v>
+      <c r="B21" s="8">
+        <f>0.0021708051*1000</f>
+        <v>2.1708050999999999</v>
       </c>
       <c r="C21" s="3">
         <v>34</v>
@@ -998,8 +1035,9 @@
       <c r="D21" s="3">
         <v>10.82277</v>
       </c>
-      <c r="E21" s="9">
-        <v>2.0009327999999998E-3</v>
+      <c r="E21" s="8">
+        <f>0.0020009328*1000</f>
+        <v>2.0009327999999997</v>
       </c>
       <c r="F21" s="3">
         <v>34</v>
@@ -1007,8 +1045,9 @@
       <c r="G21" s="3">
         <v>10.81349</v>
       </c>
-      <c r="H21" s="9">
-        <v>1.5388403E-3</v>
+      <c r="H21" s="8">
+        <f>0.0015388403*1000</f>
+        <v>1.5388402999999999</v>
       </c>
       <c r="I21" s="3">
         <v>5</v>

</xml_diff>